<commit_message>
Update 15 mar 2023
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKAKT107-001 - Akuntansi - Transaksi - SJS - Cek Jurnal Fixed income.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKAKT107-001 - Akuntansi - Transaksi - SJS - Cek Jurnal Fixed income.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Excel DPLK Newest akuntansi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DPLK 2\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AD9BB6A-62C5-4AE6-A772-4E074161FFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DPLKAKT107-001" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -107,11 +108,14 @@
   <si>
     <t>DTOBL202300007</t>
   </si>
+  <si>
+    <t>CLM202330017</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -505,11 +509,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -586,9 +590,6 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="75">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
@@ -635,9 +636,6 @@
       <c r="T2" s="6"/>
     </row>
     <row r="3" spans="1:20" ht="75">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -683,10 +681,43 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
     </row>
-    <row r="4" spans="1:20">
-      <c r="B4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+    <row r="4" spans="1:20" ht="75">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="4">
+        <v>32660</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:20">
       <c r="B5" s="2"/>

</xml_diff>